<commit_message>
replace recall rate with discover rate
</commit_message>
<xml_diff>
--- a/spring-2019/2/code/results/windows_new.xlsx
+++ b/spring-2019/2/code/results/windows_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricciwoo/Downloads/HPBDS/Project/E599-high-performance-big-data/spring-2019/2/code/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790DC21D-BABC-A44E-B1B0-738EB09962CB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC24C67-D3DB-564A-BF1C-AD97D8EAB386}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18260" windowHeight="14660" xr2:uid="{152E3284-0501-C645-A6D7-12A35F328FF7}"/>
+    <workbookView xWindow="10160" yWindow="2080" windowWidth="18260" windowHeight="14660" xr2:uid="{152E3284-0501-C645-A6D7-12A35F328FF7}"/>
   </bookViews>
   <sheets>
     <sheet name="car 1" sheetId="3" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="14">
   <si>
     <t xml:space="preserve"> Numenta HTM</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>false positive</t>
+  </si>
+  <si>
+    <t>discover rate</t>
+  </si>
+  <si>
+    <t>false positive rate</t>
   </si>
 </sst>
 </file>
@@ -202,10 +208,22 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>d</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="en-US" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>recall</a:t>
+              <a:t>is</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>cover</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" sz="2400" b="0" i="0" baseline="0">
@@ -257,6 +275,18 @@
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" sz="2400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>rate</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t> </a:t>
@@ -356,7 +386,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>recall rate</c:v>
+                  <c:v>discover rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -427,7 +457,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>false positive</c:v>
+                  <c:v>false positive rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4416,7 +4446,7 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
@@ -4429,102 +4459,102 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>recall</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="zh-CN" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>rate</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="zh-CN" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>and</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="zh-CN" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>false</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="zh-CN" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>positive</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="zh-CN" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>of</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="zh-CN" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>car</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="zh-CN" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="zh-CN" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>1</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" sz="2000" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>3</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="2000">
+            <a:endParaRPr lang="en-US" sz="2400">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -4557,7 +4587,7 @@
             <a:buFontTx/>
             <a:buNone/>
             <a:tabLst/>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
@@ -4585,11 +4615,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'car 13'!$A$29</c:f>
+              <c:f>'car 13'!$A$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>recall rate</c:v>
+                  <c:v>discover rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4656,11 +4686,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'car 13'!$A$30</c:f>
+              <c:f>'car 13'!$A$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>false positive</c:v>
+                  <c:v>false positive rate</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4764,7 +4794,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4823,7 +4853,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -4865,7 +4895,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -12238,9 +12268,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -12854,7 +12884,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B33" s="1">
         <v>0.68179999999999996</v>
@@ -12871,7 +12901,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B34" s="1">
         <v>0.51500000000000001</v>
@@ -13191,7 +13221,7 @@
   <dimension ref="A28:E69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13270,7 +13300,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B33" s="1">
         <v>0.61109999999999998</v>
@@ -13287,7 +13317,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B34" s="1">
         <v>0.27350000000000002</v>

</xml_diff>

<commit_message>
update images and slices
</commit_message>
<xml_diff>
--- a/spring-2019/2/code/results/windows_new.xlsx
+++ b/spring-2019/2/code/results/windows_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ricciwoo/Downloads/HPBDS/Project/E599-high-performance-big-data/spring-2019/2/code/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC24C67-D3DB-564A-BF1C-AD97D8EAB386}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1466F9-EBE4-E342-B733-6DE0BCAF2B50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10160" yWindow="2080" windowWidth="18260" windowHeight="14660" xr2:uid="{152E3284-0501-C645-A6D7-12A35F328FF7}"/>
+    <workbookView xWindow="10160" yWindow="2080" windowWidth="18260" windowHeight="14660" activeTab="1" xr2:uid="{152E3284-0501-C645-A6D7-12A35F328FF7}"/>
   </bookViews>
   <sheets>
     <sheet name="car 1" sheetId="3" r:id="rId1"/>
@@ -4459,10 +4459,10 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="2400" b="0" i="0" baseline="0">
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>recall</a:t>
+              <a:t>discover</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" sz="2400" b="0" i="0" baseline="0">
@@ -4517,6 +4517,12 @@
                 <a:effectLst/>
               </a:rPr>
               <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>rate </a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="2400" b="0" i="0" baseline="0">
@@ -11946,7 +11952,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -12268,7 +12274,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -12804,8 +12810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D3A623-A160-5D4A-B877-08100F29EC6E}">
   <dimension ref="A28:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13220,8 +13226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF66EA4D-CD89-EF4C-A9F2-70333253A131}">
   <dimension ref="A28:E69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>